<commit_message>
Update SOHP Excel template
</commit_message>
<xml_diff>
--- a/DCR_MODS_templates/ExceltoMODSWF/sohp_mods_template.xlsx
+++ b/DCR_MODS_templates/ExceltoMODSWF/sohp_mods_template.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\goslen\Desktop\dcr_mods_templates\2021-prefix-check\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\goslen\Git\Metadata-Miscellany\DCR_MODS_templates\ExceltoMODSWF\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D028982-5C09-4FB6-9880-EE727293835E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1201EB74-F0ED-4A96-B39C-0B36532A2C47}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="300" yWindow="210" windowWidth="27930" windowHeight="14925" xr2:uid="{728CFF79-6BFC-4A88-93FA-FB32B9BF7D29}"/>
+    <workbookView xWindow="1050" yWindow="1230" windowWidth="28515" windowHeight="13200" xr2:uid="{728CFF79-6BFC-4A88-93FA-FB32B9BF7D29}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="23">
   <si>
     <t>&lt;object pid="</t>
   </si>
@@ -50,9 +50,6 @@
     <t>Date Created</t>
   </si>
   <si>
-    <t>Identifier</t>
-  </si>
-  <si>
     <t>Interview Number</t>
   </si>
   <si>
@@ -80,22 +77,28 @@
     <t>&lt;/mods:dateCreated&gt;&lt;/mods:originInfo&gt;</t>
   </si>
   <si>
-    <t>&lt;mods:identifier type="local"&gt;</t>
-  </si>
-  <si>
     <t>&lt;/mods:identifier&gt;</t>
   </si>
   <si>
-    <t>&lt;mods:note displayLabel="Interview Number"&gt;</t>
-  </si>
-  <si>
-    <t>&lt;/mods:note&gt;</t>
-  </si>
-  <si>
-    <t>&lt;mods:typeOfResource&gt;sound recording-nonmusical&lt;/mods:typeOfResource&gt;</t>
-  </si>
-  <si>
     <t>&lt;/mods:mods&gt;&lt;/update&gt;&lt;/object&gt;</t>
+  </si>
+  <si>
+    <t>&lt;/mods:namePart&gt;</t>
+  </si>
+  <si>
+    <t>&lt;mods:namePart type="date"&gt;</t>
+  </si>
+  <si>
+    <t>Interviewee Date</t>
+  </si>
+  <si>
+    <t>Interviewer Date</t>
+  </si>
+  <si>
+    <t>&lt;mods:identifier displayLabel="Interview Number" type="local"&gt;</t>
+  </si>
+  <si>
+    <t>&lt;mods:typeOfResource&gt;sound recording-nonmusical&lt;/mods:typeOfResource&gt;&lt;mods:genre authority="lcgft"&gt;Oral histories&lt;/mods:genre&gt;</t>
   </si>
 </sst>
 </file>
@@ -153,13 +156,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -474,9 +476,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F5641A8D-7ACA-4BF9-AD80-A3884A40277A}">
-  <dimension ref="A1:W1"/>
+  <dimension ref="A1:Z1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="Z1" sqref="Z1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -484,80 +488,89 @@
     <col min="5" max="5" width="20.28515625" customWidth="1"/>
     <col min="8" max="8" width="16.42578125" customWidth="1"/>
     <col min="11" max="11" width="24.42578125" customWidth="1"/>
-    <col min="14" max="14" width="18" style="4" customWidth="1"/>
+    <col min="14" max="14" width="18" style="1" customWidth="1"/>
     <col min="17" max="17" width="16.28515625" customWidth="1"/>
     <col min="20" max="20" width="18.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" s="2" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:26" s="2" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="E1" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="H1" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="I1" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="E1" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="F1" s="2" t="s">
+      <c r="J1" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="K1" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="L1" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="M1" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="N1" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="O1" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="G1" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="H1" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="I1" s="2" t="s">
+      <c r="P1" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="Q1" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="R1" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="K1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="L1" s="2" t="s">
+      <c r="S1" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="M1" s="2" t="s">
+      <c r="T1" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="U1" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="N1" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="O1" s="2" t="s">
+      <c r="V1" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="W1" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="X1" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="P1" s="2" t="s">
+      <c r="Y1" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="Z1" s="2" t="s">
         <v>16</v>
-      </c>
-      <c r="Q1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="R1" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="S1" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="T1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="U1" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="V1" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="W1" s="2" t="s">
-        <v>21</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update sohp date encoding in spreadsheet template
</commit_message>
<xml_diff>
--- a/DCR_MODS_templates/ExceltoMODSWF/sohp_mods_template.xlsx
+++ b/DCR_MODS_templates/ExceltoMODSWF/sohp_mods_template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\goslen\Git\Metadata-Miscellany\DCR_MODS_templates\ExceltoMODSWF\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8426100-CC69-4F8D-9DC1-8C50C0A21D3D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C38A02D-2681-47F8-8645-A9757F95681F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1755" yWindow="555" windowWidth="25845" windowHeight="13845" xr2:uid="{728CFF79-6BFC-4A88-93FA-FB32B9BF7D29}"/>
+    <workbookView xWindow="2445" yWindow="1260" windowWidth="23250" windowHeight="12570" xr2:uid="{728CFF79-6BFC-4A88-93FA-FB32B9BF7D29}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -68,9 +68,6 @@
     <t>&lt;/mods:title&gt;&lt;/mods:titleInfo&gt;</t>
   </si>
   <si>
-    <t>&lt;mods:originInfo&gt;&lt;mods:dateCreated encoding="iso8601"&gt;</t>
-  </si>
-  <si>
     <t>&lt;/mods:dateCreated&gt;&lt;/mods:originInfo&gt;</t>
   </si>
   <si>
@@ -99,6 +96,9 @@
   </si>
   <si>
     <t>"&gt;&lt;datastream type="md_descriptive" operation="update"&gt;&lt;mods:mods xmlns:mods="http://www.loc.gov/mods/v3" xmlns:xlink="http://www.w3.org/1999/xlink"&gt;</t>
+  </si>
+  <si>
+    <t>&lt;mods:originInfo&gt;&lt;mods:dateCreated encoding="w3cdtf"&gt;</t>
   </si>
 </sst>
 </file>
@@ -478,8 +478,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F5641A8D-7ACA-4BF9-AD80-A3884A40277A}">
   <dimension ref="A1:Z1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
+      <selection activeCell="S1" sqref="S1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -501,7 +501,7 @@
         <v>1</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D1" s="2" t="s">
         <v>7</v>
@@ -510,13 +510,13 @@
         <v>3</v>
       </c>
       <c r="F1" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="G1" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="H1" s="4" t="s">
         <v>16</v>
-      </c>
-      <c r="H1" s="4" t="s">
-        <v>17</v>
       </c>
       <c r="I1" s="2" t="s">
         <v>8</v>
@@ -528,13 +528,13 @@
         <v>4</v>
       </c>
       <c r="L1" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="M1" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="M1" s="2" t="s">
-        <v>16</v>
-      </c>
       <c r="N1" s="4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="O1" s="2" t="s">
         <v>9</v>
@@ -549,28 +549,28 @@
         <v>11</v>
       </c>
       <c r="S1" s="2" t="s">
-        <v>12</v>
+        <v>22</v>
       </c>
       <c r="T1" s="3" t="s">
         <v>5</v>
       </c>
       <c r="U1" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="V1" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="W1" s="3" t="s">
         <v>6</v>
       </c>
       <c r="X1" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="Y1" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="Z1" s="2" t="s">
         <v>20</v>
-      </c>
-      <c r="Z1" s="2" t="s">
-        <v>21</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update SOHP excel file
</commit_message>
<xml_diff>
--- a/DCR_MODS_templates/ExceltoMODSWF/sohp_mods_template.xlsx
+++ b/DCR_MODS_templates/ExceltoMODSWF/sohp_mods_template.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\goslen\Git\Metadata-Miscellany\DCR_MODS_templates\ExceltoMODSWF\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\goslen\Downloads\copy_sohp_templates_20220518\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C38A02D-2681-47F8-8645-A9757F95681F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D90B1CE-6723-40CA-97C2-0B51E479F4E6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2445" yWindow="1260" windowWidth="23250" windowHeight="12570" xr2:uid="{728CFF79-6BFC-4A88-93FA-FB32B9BF7D29}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{728CFF79-6BFC-4A88-93FA-FB32B9BF7D29}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="39">
   <si>
     <t>&lt;object pid="</t>
   </si>
@@ -41,12 +41,6 @@
     <t>Title</t>
   </si>
   <si>
-    <t>Interviewee</t>
-  </si>
-  <si>
-    <t>Interviewer</t>
-  </si>
-  <si>
     <t>Date Created</t>
   </si>
   <si>
@@ -80,12 +74,6 @@
     <t>&lt;mods:namePart type="date"&gt;</t>
   </si>
   <si>
-    <t>Interviewee Date</t>
-  </si>
-  <si>
-    <t>Interviewer Date</t>
-  </si>
-  <si>
     <t>&lt;mods:identifier displayLabel="Interview Number" type="local"&gt;</t>
   </si>
   <si>
@@ -99,6 +87,66 @@
   </si>
   <si>
     <t>&lt;mods:originInfo&gt;&lt;mods:dateCreated encoding="w3cdtf"&gt;</t>
+  </si>
+  <si>
+    <t>Interviewee 1</t>
+  </si>
+  <si>
+    <t>Interviewee 1 Date</t>
+  </si>
+  <si>
+    <t>Interviewee 2</t>
+  </si>
+  <si>
+    <t>Interviewee 2 Date</t>
+  </si>
+  <si>
+    <t>Interviewee 3</t>
+  </si>
+  <si>
+    <t>Interviewee 3 Date</t>
+  </si>
+  <si>
+    <t>Interviewee 4</t>
+  </si>
+  <si>
+    <t>Interviewee 4 Date</t>
+  </si>
+  <si>
+    <t>Interviewee 5</t>
+  </si>
+  <si>
+    <t>Interviewee 5 Date</t>
+  </si>
+  <si>
+    <t>Interviewer 1</t>
+  </si>
+  <si>
+    <t>Interviewer 1 Date</t>
+  </si>
+  <si>
+    <t>Interviewer 2</t>
+  </si>
+  <si>
+    <t>Interviewer 2 Date</t>
+  </si>
+  <si>
+    <t>Interviewer 3</t>
+  </si>
+  <si>
+    <t>Interviewer 3 Date</t>
+  </si>
+  <si>
+    <t>Interviewer 4</t>
+  </si>
+  <si>
+    <t>Interviewer 4 Date</t>
+  </si>
+  <si>
+    <t>Interviewer 5</t>
+  </si>
+  <si>
+    <t>Interviewer 5 Date</t>
   </si>
 </sst>
 </file>
@@ -476,24 +524,41 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F5641A8D-7ACA-4BF9-AD80-A3884A40277A}">
-  <dimension ref="A1:Z1"/>
+  <dimension ref="A1:BV1"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
-      <selection activeCell="S1" sqref="S1"/>
+    <sheetView tabSelected="1" topLeftCell="BA1" workbookViewId="0">
+      <selection activeCell="BS10" sqref="BS10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="13.5703125" customWidth="1"/>
-    <col min="5" max="5" width="20.28515625" customWidth="1"/>
-    <col min="8" max="8" width="16.42578125" customWidth="1"/>
-    <col min="11" max="11" width="24.42578125" customWidth="1"/>
-    <col min="14" max="14" width="18" style="1" customWidth="1"/>
-    <col min="17" max="17" width="16.28515625" customWidth="1"/>
-    <col min="20" max="20" width="18.5703125" customWidth="1"/>
+    <col min="5" max="5" width="20.42578125" customWidth="1"/>
+    <col min="8" max="8" width="20.42578125" customWidth="1"/>
+    <col min="11" max="11" width="20.42578125" customWidth="1"/>
+    <col min="14" max="14" width="20.42578125" customWidth="1"/>
+    <col min="17" max="17" width="20.42578125" customWidth="1"/>
+    <col min="20" max="20" width="20.42578125" customWidth="1"/>
+    <col min="23" max="23" width="20.42578125" customWidth="1"/>
+    <col min="26" max="26" width="20.42578125" customWidth="1"/>
+    <col min="29" max="29" width="20.42578125" customWidth="1"/>
+    <col min="32" max="32" width="20.42578125" customWidth="1"/>
+    <col min="35" max="35" width="20.42578125" customWidth="1"/>
+    <col min="38" max="38" width="20.42578125" style="1" customWidth="1"/>
+    <col min="41" max="41" width="20.42578125" customWidth="1"/>
+    <col min="44" max="44" width="20.42578125" customWidth="1"/>
+    <col min="47" max="47" width="20.42578125" customWidth="1"/>
+    <col min="50" max="50" width="20.42578125" customWidth="1"/>
+    <col min="53" max="53" width="20.42578125" customWidth="1"/>
+    <col min="56" max="56" width="20.42578125" customWidth="1"/>
+    <col min="59" max="59" width="20.42578125" customWidth="1"/>
+    <col min="62" max="62" width="20.42578125" customWidth="1"/>
+    <col min="65" max="65" width="16.28515625" customWidth="1"/>
+    <col min="68" max="68" width="19.42578125" customWidth="1"/>
+    <col min="71" max="71" width="19.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" s="2" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:74" s="2" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -501,76 +566,220 @@
         <v>1</v>
       </c>
       <c r="C1" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="H1" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="K1" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="L1" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="M1" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="N1" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="O1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="P1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="Q1" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="R1" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="S1" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="T1" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="U1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="V1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="W1" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="X1" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="Y1" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="Z1" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="AA1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="AB1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="AC1" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="AD1" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="AE1" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="AF1" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="AG1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="AH1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="AI1" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="AJ1" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="AK1" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="AL1" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="AM1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="AN1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="AO1" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="AP1" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="AQ1" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="AR1" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="AS1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="AT1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="AU1" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="AV1" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="AW1" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="AX1" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="AY1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="AZ1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="BA1" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="BB1" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="BC1" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="BD1" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="BE1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="BF1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="BG1" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="BH1" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="BI1" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="BJ1" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="BK1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="BL1" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="BM1" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="BN1" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="BO1" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="BP1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="BQ1" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="BR1" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="BS1" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="BT1" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="BU1" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="H1" s="4" t="s">
+      <c r="BV1" s="2" t="s">
         <v>16</v>
-      </c>
-      <c r="I1" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="J1" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="K1" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="L1" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="M1" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="N1" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="O1" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="P1" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="Q1" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="R1" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="S1" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="T1" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="U1" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="V1" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="W1" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="X1" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="Y1" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="Z1" s="2" t="s">
-        <v>20</v>
       </c>
     </row>
   </sheetData>

</xml_diff>